<commit_message>
added species and updated data import to use species mapping file
</commit_message>
<xml_diff>
--- a/data/species_mapping.xlsx
+++ b/data/species_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCI\migration-maps\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C26B070-A5E7-4C1F-88CB-20820AFC21B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67171E76-15B9-4D1E-973C-5A59587E6E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plot parameters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="353">
   <si>
     <t>PLOT.NO</t>
   </si>
@@ -1079,6 +1079,12 @@
   </si>
   <si>
     <t>Glen Fergus</t>
+  </si>
+  <si>
+    <t>Rusty-tailed Flycatcher</t>
+  </si>
+  <si>
+    <t>Pied Thrush</t>
   </si>
 </sst>
 </file>
@@ -1419,21 +1425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1621,7 +1627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1679,7 +1685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1789,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1833,7 +1839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1855,7 +1861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1899,7 +1905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -2139,7 +2145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -2164,7 +2170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -2311,7 +2317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -2355,7 +2361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -2467,7 +2473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -2509,7 +2515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -2579,7 +2585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -2635,7 +2641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -2649,7 +2655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -2747,7 +2753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -2817,7 +2823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -2887,7 +2893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -2929,7 +2935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -2943,7 +2949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -2957,7 +2963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -2971,7 +2977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -3030,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -3047,7 +3053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -3064,7 +3070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -3163,6 +3169,28 @@
         <v>0</v>
       </c>
       <c r="E136" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="5">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>351</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="5">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>352</v>
+      </c>
+      <c r="E138" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3181,14 +3209,14 @@
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3202,7 +3230,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3213,7 +3241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3224,7 +3252,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3238,7 +3266,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3252,7 +3280,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3263,7 +3291,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3274,7 +3302,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3288,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3299,7 +3327,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3310,7 +3338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3321,7 +3349,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3335,7 +3363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3346,7 +3374,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3357,7 +3385,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3368,7 +3396,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3382,7 +3410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3396,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3407,7 +3435,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3418,7 +3446,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3429,7 +3457,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3440,7 +3468,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3451,7 +3479,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3462,7 +3490,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3473,7 +3501,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3484,7 +3512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -3495,7 +3523,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -3506,7 +3534,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3517,7 +3545,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -3528,7 +3556,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -3539,7 +3567,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -3550,14 +3578,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3571,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3582,7 +3610,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -3593,7 +3621,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3604,7 +3632,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -3615,7 +3643,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -3626,7 +3654,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -3637,7 +3665,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3648,7 +3676,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3662,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3673,7 +3701,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3684,7 +3712,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -3695,7 +3723,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -3706,7 +3734,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -3720,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -3731,7 +3759,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -3742,7 +3770,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3753,7 +3781,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -3764,7 +3792,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3775,7 +3803,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -3786,7 +3814,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -3797,7 +3825,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -3808,7 +3836,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -3819,7 +3847,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -3830,7 +3858,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3841,7 +3869,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -3852,7 +3880,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3863,7 +3891,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3874,7 +3902,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3885,7 +3913,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3896,7 +3924,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -3910,7 +3938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -3924,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -3935,7 +3963,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -3946,7 +3974,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -3957,7 +3985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -3971,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -3982,7 +4010,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3996,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -4007,7 +4035,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -4018,7 +4046,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -4029,7 +4057,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -4040,7 +4068,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -4051,7 +4079,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -4065,7 +4093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -4076,7 +4104,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -4087,7 +4115,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -4098,7 +4126,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -4109,7 +4137,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -4120,21 +4148,21 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>89</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>90</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -4145,7 +4173,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -4156,7 +4184,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -4167,7 +4195,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -4178,7 +4206,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -4189,7 +4217,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -4200,7 +4228,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -4211,7 +4239,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -4222,7 +4250,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -4233,7 +4261,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -4244,7 +4272,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -4255,7 +4283,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -4266,7 +4294,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -4277,7 +4305,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -4288,7 +4316,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -4299,7 +4327,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -4310,7 +4338,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -4321,7 +4349,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -4332,7 +4360,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -4343,7 +4371,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -4354,7 +4382,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -4365,7 +4393,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -4376,7 +4404,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>72</v>
       </c>
@@ -4387,7 +4415,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4398,7 +4426,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4409,7 +4437,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -4420,7 +4448,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4431,7 +4459,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -4442,7 +4470,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -4453,7 +4481,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -4464,7 +4492,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -4475,7 +4503,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -4486,7 +4514,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -4497,7 +4525,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -4508,7 +4536,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -4519,7 +4547,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -4530,7 +4558,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -4541,7 +4569,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4552,7 +4580,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -4563,7 +4591,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -4574,7 +4602,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -4585,7 +4613,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -4596,7 +4624,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -4607,7 +4635,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -4618,7 +4646,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -4629,7 +4657,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
Map zoom adjusted along with other things.
</commit_message>
<xml_diff>
--- a/data/species_mapping.xlsx
+++ b/data/species_mapping.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Plot parameters" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Species parameters" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Plot parameters'!$A$1:$G$141</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1264,28 +1261,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1296,19 +1272,19 @@
   <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.58"/>
@@ -1384,18 +1360,7 @@
       <c r="I2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>-35</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>145</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="M2" s="4" t="n">
-        <v>-18</v>
-      </c>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1423,18 +1388,7 @@
       <c r="I3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>-18</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>74</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>-170</v>
-      </c>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1459,20 +1413,9 @@
         <v>20</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>-12</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>138</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="M4" s="4" t="n">
-        <v>35</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1499,18 +1442,7 @@
       <c r="I5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>-11</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>145</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>51.7</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1537,18 +1469,6 @@
       <c r="I6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>-56.5</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>157.5</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>-143</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1575,18 +1495,7 @@
       <c r="I7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>148</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="M7" s="4" t="n">
-        <v>53</v>
-      </c>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1692,7 +1601,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -1746,7 +1655,7 @@
         <v>20</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="4"/>
     </row>
@@ -1764,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>16</v>
@@ -1794,13 +1703,13 @@
         <v>16</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M15" s="4"/>
     </row>
@@ -1859,18 +1768,7 @@
       <c r="I17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>-45</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>172</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="M17" s="4" t="n">
-        <v>-30</v>
-      </c>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1922,7 +1820,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M19" s="4"/>
     </row>
@@ -1949,7 +1847,7 @@
         <v>20</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M20" s="4"/>
     </row>
@@ -2003,7 +1901,7 @@
         <v>20</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M22" s="4"/>
     </row>
@@ -2090,7 +1988,7 @@
         <v>17</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M25" s="4"/>
     </row>
@@ -2198,7 +2096,7 @@
         <v>20</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M29" s="4"/>
     </row>
@@ -2246,13 +2144,13 @@
         <v>16</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M31" s="4"/>
     </row>
@@ -2387,7 +2285,7 @@
         <v>16</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>17</v>
@@ -2447,7 +2345,7 @@
         <v>17</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,7 +2362,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>16</v>
@@ -2473,7 +2371,7 @@
         <v>17</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M39" s="4"/>
     </row>
@@ -2638,7 +2536,7 @@
         <v>17</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M45" s="4"/>
     </row>
@@ -2741,7 +2639,7 @@
         <v>15</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49" s="0" t="s">
         <v>17</v>
@@ -2765,10 +2663,10 @@
         <v>14</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H50" s="0" t="s">
         <v>17</v>
@@ -2795,7 +2693,7 @@
         <v>15</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="0" t="s">
         <v>17</v>
@@ -2855,7 +2753,7 @@
         <v>17</v>
       </c>
       <c r="I53" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M53" s="4"/>
     </row>
@@ -2879,7 +2777,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" s="0" t="s">
         <v>20</v>
@@ -2934,7 +2832,7 @@
         <v>16</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H56" s="0" t="s">
         <v>17</v>
@@ -3021,7 +2919,7 @@
         <v>17</v>
       </c>
       <c r="I59" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M59" s="4"/>
     </row>
@@ -3048,7 +2946,7 @@
         <v>17</v>
       </c>
       <c r="I60" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M60" s="4"/>
     </row>
@@ -3102,7 +3000,7 @@
         <v>20</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M62" s="4"/>
     </row>
@@ -3123,13 +3021,13 @@
         <v>16</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H63" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I63" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M63" s="4"/>
     </row>
@@ -3156,7 +3054,7 @@
         <v>17</v>
       </c>
       <c r="I64" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M64" s="4"/>
     </row>
@@ -3352,11 +3250,6 @@
       <c r="M71" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G141">
-    <sortState ref="A2:G141">
-      <sortCondition ref="A2:A141" customList=""/>
-    </sortState>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3364,7 +3257,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3379,7 +3271,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>

</xml_diff>